<commit_message>
Once again for member
</commit_message>
<xml_diff>
--- a/HCHNAexcelFiles/MEMBER.xlsx
+++ b/HCHNAexcelFiles/MEMBER.xlsx
@@ -819,9 +819,9 @@
   <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -876,9 +876,6 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
       <c r="B2" s="1" t="s">
         <v>144</v>
       </c>
@@ -893,9 +890,6 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
       <c r="B3" s="1" t="s">
         <v>144</v>
       </c>
@@ -910,9 +904,6 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
       <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
@@ -927,9 +918,6 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
@@ -944,9 +932,6 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
       <c r="B6" s="1" t="s">
         <v>141</v>
       </c>
@@ -964,9 +949,6 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
@@ -981,9 +963,6 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
@@ -998,9 +977,6 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1015,9 +991,6 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1032,9 +1005,6 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
       <c r="B11" s="1" t="s">
         <v>142</v>
       </c>
@@ -1052,9 +1022,6 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
       <c r="B12" s="1" t="s">
         <v>142</v>
       </c>
@@ -1072,9 +1039,6 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1089,9 +1053,6 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1106,9 +1067,6 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1123,9 +1081,6 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
       <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
@@ -1139,10 +1094,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1156,10 +1108,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1173,10 +1122,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1190,10 +1136,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
@@ -1207,10 +1150,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>31</v>
       </c>
@@ -1224,10 +1164,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1241,10 +1178,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1267,10 +1201,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1290,10 +1221,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>145</v>
       </c>
@@ -1307,10 +1235,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1324,10 +1249,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -1341,10 +1263,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
@@ -1358,10 +1277,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>146</v>
       </c>
@@ -1375,10 +1291,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>146</v>
       </c>
@@ -1392,10 +1305,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>143</v>
       </c>
@@ -1409,10 +1319,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>15</v>
       </c>
@@ -1426,10 +1333,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1443,10 +1347,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1460,10 +1361,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>22</v>
       </c>
@@ -1477,10 +1375,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>22</v>
       </c>
@@ -1494,10 +1389,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>10</v>
       </c>
@@ -1514,10 +1406,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>21</v>
       </c>
@@ -1534,10 +1423,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>70</v>
       </c>
@@ -1551,10 +1437,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>70</v>
       </c>
@@ -1568,10 +1451,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>16</v>
       </c>
@@ -1588,10 +1468,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1605,10 +1482,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>12</v>
       </c>
@@ -1622,10 +1496,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>23</v>
       </c>
@@ -1639,10 +1510,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>23</v>
       </c>
@@ -1659,10 +1527,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1694,10 +1559,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>90</v>
       </c>
@@ -1729,10 +1591,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>8</v>
       </c>
@@ -1749,10 +1608,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>43</v>
       </c>
@@ -1769,10 +1625,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>16</v>
       </c>
@@ -1786,10 +1639,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>13</v>
       </c>
@@ -1803,10 +1653,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>51</v>
-      </c>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>10</v>
       </c>
@@ -1820,10 +1667,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>9</v>
       </c>
@@ -1837,10 +1681,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>53</v>
-      </c>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>